<commit_message>
inital commit for pysr, edits R script for correct files, and edits chemical names due to pysr restrictions
</commit_message>
<xml_diff>
--- a/LK_Prelim_Model/ChemistrywTox_MouseMap_042821.xlsx
+++ b/LK_Prelim_Model/ChemistrywTox_MouseMap_042821.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliarager/Library/CloudStorage/OneDrive-UniversityofNorthCarolinaatChapelHill/Shared_Grants/2024/NIH_Suppl_Cloud_2024/7_Preliminary Analyses/Wildfire Mouse Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Desktop/wildfire/NIH_Cloud_NOSI/LK_Prelim_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A8072E-3B4A-504E-B4C1-B36DD14BEB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB364041-1732-A845-BB39-F1C1A9B9715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48920" yWindow="500" windowWidth="46260" windowHeight="25880" xr2:uid="{E9D93C69-1D32-7543-A0FD-2FB11E5159CA}"/>
+    <workbookView xWindow="0" yWindow="4380" windowWidth="29920" windowHeight="18660" xr2:uid="{E9D93C69-1D32-7543-A0FD-2FB11E5159CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="325">
   <si>
     <t>Measure</t>
   </si>
@@ -960,6 +960,60 @@
   </si>
   <si>
     <t>M140</t>
+  </si>
+  <si>
+    <t>Benzaanthracene</t>
+  </si>
+  <si>
+    <t>Benzoapyrene</t>
+  </si>
+  <si>
+    <t>Benzobfluoranthene</t>
+  </si>
+  <si>
+    <t>Benzoepyrene</t>
+  </si>
+  <si>
+    <t>Benzokfluoranthene</t>
+  </si>
+  <si>
+    <t>Benzoghiperylene</t>
+  </si>
+  <si>
+    <t>Indeno123cdpyrene</t>
+  </si>
+  <si>
+    <t>Potassium</t>
+  </si>
+  <si>
+    <t>Sulfur</t>
+  </si>
+  <si>
+    <t>Silicon</t>
+  </si>
+  <si>
+    <t>Methylnonadecane2</t>
+  </si>
+  <si>
+    <t>Methylnonadecane3</t>
+  </si>
+  <si>
+    <t>Methylchysene1</t>
+  </si>
+  <si>
+    <t>Methylnaphthalene1</t>
+  </si>
+  <si>
+    <t>Methylnaphthalene2</t>
+  </si>
+  <si>
+    <t>Dimethylnaphthalene26</t>
+  </si>
+  <si>
+    <t>Methylanthracene9</t>
+  </si>
+  <si>
+    <t>Dimethoxyphenol35</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1023,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1074,9 +1128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1114,7 +1168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1220,7 +1274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1362,7 +1416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1373,81 +1427,81 @@
   <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="8" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="13" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1461,9 +1515,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>317</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1475,9 +1529,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>318</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -1489,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1503,7 +1557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1517,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1531,7 +1585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1545,7 +1599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1559,7 +1613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1573,7 +1627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1587,7 +1641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1601,7 +1655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1615,7 +1669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1629,7 +1683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1643,7 +1697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1657,7 +1711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1671,7 +1725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1685,7 +1739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1699,7 +1753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1713,7 +1767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1727,7 +1781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1741,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -1755,7 +1809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -1769,7 +1823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -1783,7 +1837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
@@ -1797,7 +1851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -1811,9 +1865,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>32</v>
+        <v>319</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -1825,9 +1879,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>34</v>
+        <v>320</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1839,9 +1893,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>35</v>
+        <v>321</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1853,9 +1907,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>36</v>
+        <v>322</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1867,9 +1921,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>37</v>
+        <v>323</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1881,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
@@ -1895,7 +1949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -1909,9 +1963,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>40</v>
+        <v>307</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
@@ -1923,9 +1977,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>308</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -1937,9 +1991,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>42</v>
+        <v>309</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -1951,9 +2005,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>5</v>
@@ -1965,9 +2019,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>44</v>
+        <v>311</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>5</v>
@@ -1979,9 +2033,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>45</v>
+        <v>312</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
@@ -1993,7 +2047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -2007,7 +2061,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>47</v>
       </c>
@@ -2021,7 +2075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -2035,7 +2089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>49</v>
       </c>
@@ -2049,9 +2103,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>50</v>
+        <v>313</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2063,7 +2117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>51</v>
       </c>
@@ -2077,7 +2131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>52</v>
       </c>
@@ -2091,7 +2145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
@@ -2105,7 +2159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>54</v>
       </c>
@@ -2119,7 +2173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>55</v>
       </c>
@@ -2133,7 +2187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -2147,9 +2201,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>57</v>
+        <v>324</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2161,7 +2215,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -2175,7 +2229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>60</v>
       </c>
@@ -2189,7 +2243,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>61</v>
       </c>
@@ -2203,7 +2257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
@@ -2217,7 +2271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -2231,7 +2285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>64</v>
       </c>
@@ -2245,7 +2299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>65</v>
       </c>
@@ -2259,7 +2313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>66</v>
       </c>
@@ -2273,7 +2327,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>67</v>
       </c>
@@ -2287,7 +2341,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -2301,7 +2355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>69</v>
       </c>
@@ -2315,7 +2369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>70</v>
       </c>
@@ -2329,7 +2383,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>73</v>
       </c>
@@ -2343,7 +2397,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -2357,7 +2411,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -2371,7 +2425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -2385,7 +2439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -2399,7 +2453,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -2413,9 +2467,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>79</v>
+        <v>314</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>71</v>
@@ -2427,7 +2481,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>80</v>
       </c>
@@ -2441,7 +2495,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2455,7 +2509,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2469,7 +2523,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2483,7 +2537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2497,7 +2551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2511,9 +2565,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>86</v>
+        <v>315</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>71</v>
@@ -2525,7 +2579,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -2539,9 +2593,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>88</v>
+        <v>316</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>71</v>
@@ -2553,7 +2607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -2567,7 +2621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -2581,7 +2635,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -2595,7 +2649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -2609,7 +2663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>95</v>
       </c>
@@ -2623,7 +2677,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>96</v>
       </c>
@@ -2637,7 +2691,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>97</v>
       </c>
@@ -2651,7 +2705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>98</v>
       </c>
@@ -2665,7 +2719,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>99</v>
       </c>
@@ -2679,7 +2733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>103</v>
       </c>
@@ -2693,7 +2747,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>104</v>
       </c>
@@ -2707,7 +2761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>105</v>
       </c>
@@ -2721,7 +2775,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>106</v>
       </c>
@@ -2735,7 +2789,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>108</v>
       </c>
@@ -2749,7 +2803,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>109</v>
       </c>
@@ -2763,7 +2817,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>110</v>
       </c>
@@ -2777,7 +2831,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>111</v>
       </c>
@@ -2791,7 +2845,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>112</v>
       </c>
@@ -2805,7 +2859,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>113</v>
       </c>
@@ -2819,7 +2873,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>115</v>
       </c>
@@ -2833,7 +2887,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>116</v>
       </c>
@@ -2847,7 +2901,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>117</v>
       </c>
@@ -2861,7 +2915,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>118</v>
       </c>
@@ -2875,7 +2929,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>119</v>
       </c>
@@ -2889,7 +2943,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>120</v>
       </c>
@@ -2903,7 +2957,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>121</v>
       </c>
@@ -2917,7 +2971,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>122</v>
       </c>
@@ -2931,7 +2985,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>123</v>
       </c>
@@ -2945,7 +2999,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>124</v>
       </c>
@@ -2959,7 +3013,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>127</v>
       </c>
@@ -2973,7 +3027,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>128</v>
       </c>
@@ -2987,7 +3041,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>129</v>
       </c>
@@ -3014,87 +3068,87 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="8" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="13" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -3138,7 +3192,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3182,7 +3236,7 @@
         <v>5.6568542494923796E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -3226,7 +3280,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3270,7 +3324,7 @@
         <v>9.1923881554251172E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -3314,7 +3368,7 @@
         <v>3.5355339059327376E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -3358,7 +3412,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3402,7 +3456,7 @@
         <v>0.12727922061357855</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -3446,7 +3500,7 @@
         <v>0.12020815280171308</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -3490,7 +3544,7 @@
         <v>0.1414213562373095</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3534,7 +3588,7 @@
         <v>0.13435028842544403</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -3578,7 +3632,7 @@
         <v>9.1923881554251172E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -3622,7 +3676,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -3666,7 +3720,7 @@
         <v>0.18384776310850234</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -3710,7 +3764,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3754,7 +3808,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -3798,7 +3852,7 @@
         <v>0.16263455967290594</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -3842,7 +3896,7 @@
         <v>5.6568542494923796E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -3886,7 +3940,7 @@
         <v>7.778174593052023E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -3930,7 +3984,7 @@
         <v>8.4852813742385694E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -3974,7 +4028,7 @@
         <v>3.5355339059327376E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -4018,7 +4072,7 @@
         <v>4.9497474683058325E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -4062,7 +4116,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -4106,7 +4160,7 @@
         <v>0.15556349186104046</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -4150,7 +4204,7 @@
         <v>9.899494936611665E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
@@ -4194,7 +4248,7 @@
         <v>0.13435028842544403</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -4238,7 +4292,7 @@
         <v>7.778174593052023E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
@@ -4282,7 +4336,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -4326,7 +4380,7 @@
         <v>0.11313708498984759</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>35</v>
       </c>
@@ -4370,7 +4424,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
@@ -4414,7 +4468,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>37</v>
       </c>
@@ -4458,7 +4512,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
@@ -4502,7 +4556,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -4546,7 +4600,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>40</v>
       </c>
@@ -4590,7 +4644,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>41</v>
       </c>
@@ -4634,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
@@ -4678,7 +4732,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>43</v>
       </c>
@@ -4722,7 +4776,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>44</v>
       </c>
@@ -4766,7 +4820,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>45</v>
       </c>
@@ -4810,7 +4864,7 @@
         <v>8.4852813742385694E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -4854,7 +4908,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>47</v>
       </c>
@@ -4898,7 +4952,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -4942,7 +4996,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>49</v>
       </c>
@@ -4986,7 +5040,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>50</v>
       </c>
@@ -5030,7 +5084,7 @@
         <v>4.9497474683058325E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>51</v>
       </c>
@@ -5074,7 +5128,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>52</v>
       </c>
@@ -5118,7 +5172,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
@@ -5162,7 +5216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>54</v>
       </c>
@@ -5206,7 +5260,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>55</v>
       </c>
@@ -5250,7 +5304,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -5294,7 +5348,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>57</v>
       </c>
@@ -5338,7 +5392,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -5382,7 +5436,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>60</v>
       </c>
@@ -5426,7 +5480,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>61</v>
       </c>
@@ -5470,7 +5524,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
@@ -5514,7 +5568,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -5558,7 +5612,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>64</v>
       </c>
@@ -5602,7 +5656,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>65</v>
       </c>
@@ -5646,7 +5700,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>66</v>
       </c>
@@ -5690,7 +5744,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>67</v>
       </c>
@@ -5734,7 +5788,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -5778,7 +5832,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>69</v>
       </c>
@@ -5822,7 +5876,7 @@
         <v>0.17677669529663687</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>70</v>
       </c>
@@ -5866,7 +5920,7 @@
         <v>0.8987327188881018</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>73</v>
       </c>
@@ -5910,7 +5964,7 @@
         <v>3.1112698372208088E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -5954,7 +6008,7 @@
         <v>1.936058366888767</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -5998,7 +6052,7 @@
         <v>2.1920310216782972E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -6042,7 +6096,7 @@
         <v>3.3234018715767734E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -6086,7 +6140,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -6130,7 +6184,7 @@
         <v>0.26870057685088805</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>79</v>
       </c>
@@ -6174,7 +6228,7 @@
         <v>0.55932146391855908</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>80</v>
       </c>
@@ -6218,7 +6272,7 @@
         <v>0.21991020894901625</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>81</v>
       </c>
@@ -6262,7 +6316,7 @@
         <v>3.3234018715767734E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>82</v>
       </c>
@@ -6306,7 +6360,7 @@
         <v>0.58194888091652852</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -6350,7 +6404,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -6394,7 +6448,7 @@
         <v>0.19940411229460636</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -6438,7 +6492,7 @@
         <v>2.9698484809834995E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>86</v>
       </c>
@@ -6482,7 +6536,7 @@
         <v>70.710678118654741</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -6526,7 +6580,7 @@
         <v>3.1819805153394637E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>88</v>
       </c>
@@ -6570,7 +6624,7 @@
         <v>3.3941125496954276</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -6614,7 +6668,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -6658,7 +6712,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -6702,7 +6756,7 @@
         <v>9.616652224137047E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -6746,7 +6800,7 @@
         <v>9.9702056147303198E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>95</v>
       </c>
@@ -6790,7 +6844,7 @@
         <v>5.12652416360247E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>96</v>
       </c>
@@ -6834,7 +6888,7 @@
         <v>5.550788232314397E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>97</v>
       </c>
@@ -6878,7 +6932,7 @@
         <v>5.3033008588990866E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>98</v>
       </c>
@@ -6933,24 +6987,24 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.375" customWidth="1"/>
-    <col min="2" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="27.875" customWidth="1"/>
-    <col min="5" max="5" width="29.375" customWidth="1"/>
-    <col min="6" max="7" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="26.5" customWidth="1"/>
-    <col min="13" max="13" width="19.375" customWidth="1"/>
-    <col min="14" max="14" width="16.125" customWidth="1"/>
-    <col min="15" max="15" width="14.125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>143</v>
       </c>
@@ -6997,7 +7051,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -7044,7 +7098,7 @@
         <v>3.1789999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>157</v>
       </c>
@@ -7091,7 +7145,7 @@
         <v>4.4740000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>157</v>
       </c>
@@ -7138,7 +7192,7 @@
         <v>3.4950000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
@@ -7169,7 +7223,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>157</v>
       </c>
@@ -7216,7 +7270,7 @@
         <v>3.847</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>157</v>
       </c>
@@ -7263,7 +7317,7 @@
         <v>2.6579999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>132</v>
       </c>
@@ -7310,7 +7364,7 @@
         <v>3.6040000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>132</v>
       </c>
@@ -7357,7 +7411,7 @@
         <v>3.6669999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>132</v>
       </c>
@@ -7404,7 +7458,7 @@
         <v>3.806</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
@@ -7451,7 +7505,7 @@
         <v>3.8879999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>132</v>
       </c>
@@ -7498,7 +7552,7 @@
         <v>4.1429999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>132</v>
       </c>
@@ -7545,7 +7599,7 @@
         <v>5.6070000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>133</v>
       </c>
@@ -7592,7 +7646,7 @@
         <v>3.9380000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>133</v>
       </c>
@@ -7639,7 +7693,7 @@
         <v>3.867</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>133</v>
       </c>
@@ -7686,7 +7740,7 @@
         <v>3.9780000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>133</v>
       </c>
@@ -7733,7 +7787,7 @@
         <v>4.0350000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>133</v>
       </c>
@@ -7780,7 +7834,7 @@
         <v>2.653</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>133</v>
       </c>
@@ -7827,7 +7881,7 @@
         <v>3.012</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>134</v>
       </c>
@@ -7874,7 +7928,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>134</v>
       </c>
@@ -7921,7 +7975,7 @@
         <v>4.2030000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>134</v>
       </c>
@@ -7968,7 +8022,7 @@
         <v>3.9649999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>134</v>
       </c>
@@ -8015,7 +8069,7 @@
         <v>2.7109999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>134</v>
       </c>
@@ -8062,7 +8116,7 @@
         <v>3.1219999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>134</v>
       </c>
@@ -8109,7 +8163,7 @@
         <v>3.3889999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>135</v>
       </c>
@@ -8156,7 +8210,7 @@
         <v>3.3730000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>135</v>
       </c>
@@ -8203,7 +8257,7 @@
         <v>3.6019999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>135</v>
       </c>
@@ -8250,7 +8304,7 @@
         <v>4.867</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>135</v>
       </c>
@@ -8297,7 +8351,7 @@
         <v>3.8439999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>135</v>
       </c>
@@ -8344,7 +8398,7 @@
         <v>3.8719999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>135</v>
       </c>
@@ -8391,7 +8445,7 @@
         <v>4.0620000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>136</v>
       </c>
@@ -8438,7 +8492,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>136</v>
       </c>
@@ -8485,7 +8539,7 @@
         <v>3.6040000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>136</v>
       </c>
@@ -8532,7 +8586,7 @@
         <v>3.7210000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
@@ -8579,7 +8633,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -8626,7 +8680,7 @@
         <v>4.1619999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>136</v>
       </c>
@@ -8673,7 +8727,7 @@
         <v>4.226</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>137</v>
       </c>
@@ -8720,7 +8774,7 @@
         <v>4.0979999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>137</v>
       </c>
@@ -8767,7 +8821,7 @@
         <v>4.1769999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>137</v>
       </c>
@@ -8814,7 +8868,7 @@
         <v>2.794</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -8861,7 +8915,7 @@
         <v>2.9740000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>137</v>
       </c>
@@ -8908,7 +8962,7 @@
         <v>3.137</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>137</v>
       </c>
@@ -8955,7 +9009,7 @@
         <v>3.2189999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>138</v>
       </c>
@@ -9002,7 +9056,7 @@
         <v>5.1280000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>138</v>
       </c>
@@ -9049,7 +9103,7 @@
         <v>4.2880000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>138</v>
       </c>
@@ -9096,7 +9150,7 @@
         <v>2.726</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>138</v>
       </c>
@@ -9143,7 +9197,7 @@
         <v>2.988</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>138</v>
       </c>
@@ -9190,7 +9244,7 @@
         <v>3.1520000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>138</v>
       </c>
@@ -9235,7 +9289,7 @@
         <v>4.8860000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>139</v>
       </c>
@@ -9282,7 +9336,7 @@
         <v>3.3959999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
@@ -9329,7 +9383,7 @@
         <v>3.4580000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>139</v>
       </c>
@@ -9376,7 +9430,7 @@
         <v>3.673</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>139</v>
       </c>
@@ -9423,7 +9477,7 @@
         <v>3.7949999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>139</v>
       </c>
@@ -9470,7 +9524,7 @@
         <v>3.9980000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>139</v>
       </c>
@@ -9517,7 +9571,7 @@
         <v>3.7309999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>140</v>
       </c>
@@ -9564,7 +9618,7 @@
         <v>2.7240000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>140</v>
       </c>
@@ -9611,7 +9665,7 @@
         <v>2.923</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>140</v>
       </c>
@@ -9658,7 +9712,7 @@
         <v>3.1829999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>140</v>
       </c>
@@ -9705,7 +9759,7 @@
         <v>3.3039999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>140</v>
       </c>
@@ -9752,7 +9806,7 @@
         <v>3.448</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>140</v>
       </c>
@@ -9799,7 +9853,7 @@
         <v>3.694</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>141</v>
       </c>
@@ -9846,7 +9900,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>141</v>
       </c>
@@ -9893,7 +9947,7 @@
         <v>3.2570000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>141</v>
       </c>
@@ -9940,7 +9994,7 @@
         <v>2.6230000000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>141</v>
       </c>
@@ -9987,7 +10041,7 @@
         <v>2.9449999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -10034,7 +10088,7 @@
         <v>3.2879999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>141</v>
       </c>
@@ -10081,7 +10135,7 @@
         <v>3.3719999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>231</v>
       </c>
@@ -10128,7 +10182,7 @@
         <v>2.8919999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>231</v>
       </c>
@@ -10175,7 +10229,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>231</v>
       </c>
@@ -10222,7 +10276,7 @@
         <v>3.3460000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>231</v>
       </c>
@@ -10283,24 +10337,24 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.375" customWidth="1"/>
-    <col min="2" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="27.875" customWidth="1"/>
-    <col min="5" max="5" width="29.375" customWidth="1"/>
-    <col min="6" max="7" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="26.5" customWidth="1"/>
-    <col min="13" max="13" width="19.375" customWidth="1"/>
-    <col min="14" max="14" width="16.125" customWidth="1"/>
-    <col min="15" max="15" width="14.125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>143</v>
       </c>
@@ -10347,7 +10401,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -10394,7 +10448,7 @@
         <v>3.5750000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>157</v>
       </c>
@@ -10441,7 +10495,7 @@
         <v>2.6880000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>157</v>
       </c>
@@ -10488,7 +10542,7 @@
         <v>3.153</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
@@ -10535,7 +10589,7 @@
         <v>3.4020000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>157</v>
       </c>
@@ -10582,7 +10636,7 @@
         <v>3.508</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>157</v>
       </c>
@@ -10629,7 +10683,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>132</v>
       </c>
@@ -10676,7 +10730,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>132</v>
       </c>
@@ -10723,7 +10777,7 @@
         <v>5.3769999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>132</v>
       </c>
@@ -10770,7 +10824,7 @@
         <v>5.891</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
@@ -10817,7 +10871,7 @@
         <v>3.2719999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>132</v>
       </c>
@@ -10864,7 +10918,7 @@
         <v>3.407</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>132</v>
       </c>
@@ -10911,7 +10965,7 @@
         <v>3.6659999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>133</v>
       </c>
@@ -10958,7 +11012,7 @@
         <v>4.3730000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>133</v>
       </c>
@@ -11005,7 +11059,7 @@
         <v>4.4470000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>133</v>
       </c>
@@ -11052,7 +11106,7 @@
         <v>4.5439999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>133</v>
       </c>
@@ -11099,7 +11153,7 @@
         <v>4.3819999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>133</v>
       </c>
@@ -11146,7 +11200,7 @@
         <v>2.8260000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>133</v>
       </c>
@@ -11193,7 +11247,7 @@
         <v>3.258</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>134</v>
       </c>
@@ -11240,7 +11294,7 @@
         <v>3.0169999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>134</v>
       </c>
@@ -11287,7 +11341,7 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>134</v>
       </c>
@@ -11334,7 +11388,7 @@
         <v>3.2759999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>134</v>
       </c>
@@ -11381,7 +11435,7 @@
         <v>3.4830000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>134</v>
       </c>
@@ -11428,7 +11482,7 @@
         <v>3.6589999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>134</v>
       </c>
@@ -11475,7 +11529,7 @@
         <v>3.8580000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>135</v>
       </c>
@@ -11522,7 +11576,7 @@
         <v>3.472</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>135</v>
       </c>
@@ -11569,7 +11623,7 @@
         <v>3.637</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>135</v>
       </c>
@@ -11616,7 +11670,7 @@
         <v>3.7669999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>135</v>
       </c>
@@ -11663,7 +11717,7 @@
         <v>3.9710000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>135</v>
       </c>
@@ -11710,7 +11764,7 @@
         <v>4.1529999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>135</v>
       </c>
@@ -11757,7 +11811,7 @@
         <v>5.4630000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>136</v>
       </c>
@@ -11804,7 +11858,7 @@
         <v>3.996</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>136</v>
       </c>
@@ -11851,7 +11905,7 @@
         <v>4.3040000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>136</v>
       </c>
@@ -11880,7 +11934,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
@@ -11927,7 +11981,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -11974,7 +12028,7 @@
         <v>2.8039999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>136</v>
       </c>
@@ -12021,7 +12075,7 @@
         <v>3.0489999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>137</v>
       </c>
@@ -12068,7 +12122,7 @@
         <v>5.5620000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>137</v>
       </c>
@@ -12115,7 +12169,7 @@
         <v>6.29</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>137</v>
       </c>
@@ -12162,7 +12216,7 @@
         <v>3.2559999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -12209,7 +12263,7 @@
         <v>3.4390000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>137</v>
       </c>
@@ -12256,7 +12310,7 @@
         <v>3.6160000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>137</v>
       </c>
@@ -12303,7 +12357,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>138</v>
       </c>
@@ -12350,7 +12404,7 @@
         <v>3.3140000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>138</v>
       </c>
@@ -12397,7 +12451,7 @@
         <v>3.5379999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>138</v>
       </c>
@@ -12444,7 +12498,7 @@
         <v>3.6480000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>138</v>
       </c>
@@ -12491,7 +12545,7 @@
         <v>3.8450000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>138</v>
       </c>
@@ -12538,7 +12592,7 @@
         <v>4.0869999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>138</v>
       </c>
@@ -12585,7 +12639,7 @@
         <v>4.2270000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>139</v>
       </c>
@@ -12632,7 +12686,7 @@
         <v>4.0279999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
@@ -12679,7 +12733,7 @@
         <v>3.6539999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>139</v>
       </c>
@@ -12726,7 +12780,7 @@
         <v>3.617</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>139</v>
       </c>
@@ -12773,7 +12827,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>139</v>
       </c>
@@ -12820,7 +12874,7 @@
         <v>3.9969999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>139</v>
       </c>
@@ -12867,7 +12921,7 @@
         <v>4.1989999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>140</v>
       </c>
@@ -12914,7 +12968,7 @@
         <v>3.8889999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>140</v>
       </c>
@@ -12961,7 +13015,7 @@
         <v>4.0709999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>140</v>
       </c>
@@ -13008,7 +13062,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>140</v>
       </c>
@@ -13055,7 +13109,7 @@
         <v>4.367</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>140</v>
       </c>
@@ -13102,7 +13156,7 @@
         <v>5.3659999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>140</v>
       </c>
@@ -13149,7 +13203,7 @@
         <v>4.1059999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>141</v>
       </c>
@@ -13196,7 +13250,7 @@
         <v>3.677</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>141</v>
       </c>
@@ -13243,7 +13297,7 @@
         <v>3.8279999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>141</v>
       </c>
@@ -13290,7 +13344,7 @@
         <v>3.9550000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>141</v>
       </c>
@@ -13337,7 +13391,7 @@
         <v>3.605</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -13384,7 +13438,7 @@
         <v>3.077</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>141</v>
       </c>
@@ -13431,7 +13485,7 @@
         <v>3.3730000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>231</v>
       </c>
@@ -13478,7 +13532,7 @@
         <v>3.9849999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>231</v>
       </c>
@@ -13525,7 +13579,7 @@
         <v>3.8980000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>231</v>
       </c>
@@ -13572,7 +13626,7 @@
         <v>3.6930000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>231</v>
       </c>
@@ -13625,6 +13679,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8DF4565409F7A498078360796F26CA9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d9fe6ba3ad0296993fdf9ca86fb8ec6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="13928eb9-0d8a-4018-8962-fa9e89967672" xmlns:ns3="d960e8a8-69e2-40a4-bb78-08ff18f8bb2f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84c00418da9684fb2e9f40c453441992" ns2:_="" ns3:_="">
     <xsd:import namespace="13928eb9-0d8a-4018-8962-fa9e89967672"/>
@@ -13879,19 +13942,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209E5E74-AAAA-4AAD-832B-22F4FC51D717}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C7EE5A2-8461-4909-A45F-0A6C43DF2417}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C7EE5A2-8461-4909-A45F-0A6C43DF2417}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209E5E74-AAAA-4AAD-832B-22F4FC51D717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="13928eb9-0d8a-4018-8962-fa9e89967672"/>
+    <ds:schemaRef ds:uri="d960e8a8-69e2-40a4-bb78-08ff18f8bb2f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update omic runs to 1500 iterations, clean up plots
</commit_message>
<xml_diff>
--- a/LK_Prelim_Model/ChemistrywTox_MouseMap_042821.xlsx
+++ b/LK_Prelim_Model/ChemistrywTox_MouseMap_042821.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Desktop/wildfire/NIH_Cloud_NOSI/LK_Prelim_Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/jrchapp3_ad_unc_edu/Documents/Symbolic_regression_github/NIH_Cloud_NOSI/LK_Prelim_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB364041-1732-A845-BB39-F1C1A9B9715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4380" windowWidth="29920" windowHeight="18660" xr2:uid="{E9D93C69-1D32-7543-A0FD-2FB11E5159CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E9D93C69-1D32-7543-A0FD-2FB11E5159CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -1426,82 +1426,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16299F68-2850-9544-905F-01EB3FA00FDC}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.875" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="8" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="13" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.375" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>317</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>318</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>319</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>320</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>321</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>322</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>323</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>307</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>308</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>309</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>310</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>311</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>312</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>47</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>49</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>313</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>51</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>52</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>54</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>55</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>324</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>60</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>61</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>64</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>65</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>66</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>67</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>69</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>70</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>73</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>314</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>80</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>315</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>316</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>95</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>96</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>97</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>98</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>99</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>103</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>104</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>105</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>106</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>108</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>109</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>110</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>111</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>112</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>113</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>115</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>116</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>117</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>118</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>119</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>120</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>121</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>122</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>123</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>124</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>127</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>128</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>129</v>
       </c>
@@ -3064,91 +3064,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75F7B8F-4A60-B044-93B5-EC9DECD67F96}">
   <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.375" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.875" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.375" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="8" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6.625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="13" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="4.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>5.6568542494923796E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>9.1923881554251172E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>3.5355339059327376E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>0.12727922061357855</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>0.12020815280171308</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>0.1414213562373095</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>0.13435028842544403</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>9.1923881554251172E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0.18384776310850234</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>0.16263455967290594</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>5.6568542494923796E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>7.778174593052023E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>8.4852813742385694E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>3.5355339059327376E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>4.9497474683058325E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>0.15556349186104046</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>9.899494936611665E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>0.13435028842544403</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>7.778174593052023E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>0.11313708498984759</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>35</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>6.3639610306789274E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>37</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>0.10606601717798211</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>40</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>41</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>43</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>44</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>45</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>8.4852813742385694E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>47</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>49</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>50</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>4.9497474683058325E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>51</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>52</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>54</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>7.0710678118654745E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>55</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>2.1213203435596423E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>57</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>60</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>61</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>62</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>64</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>65</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>66</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>67</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>69</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>0.17677669529663687</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>70</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>0.8987327188881018</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>73</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>3.1112698372208088E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>1.936058366888767</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>2.1920310216782972E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>3.3234018715767734E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>2.8284271247461898E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>0.26870057685088805</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>79</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>0.55932146391855908</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>80</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>0.21991020894901625</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>81</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>3.3234018715767734E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>82</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>0.58194888091652852</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>0.19940411229460636</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>2.9698484809834995E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>86</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>70.710678118654741</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>3.1819805153394637E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>88</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>3.3941125496954276</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>1.4142135623730949E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>4.2426406871192847E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>9.616652224137047E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>9.9702056147303198E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>95</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>5.12652416360247E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>96</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>5.550788232314397E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>97</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>5.3033008588990866E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>98</v>
       </c>
@@ -6987,24 +6987,24 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.375" customWidth="1"/>
+    <col min="2" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="27.875" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
+    <col min="6" max="7" width="17.625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
     <col min="12" max="12" width="26.5" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="19.375" customWidth="1"/>
+    <col min="14" max="14" width="16.125" customWidth="1"/>
+    <col min="15" max="15" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>143</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>3.1789999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>157</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>4.4740000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>157</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>3.4950000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
@@ -7223,7 +7223,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>157</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>3.847</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>157</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>2.6579999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>132</v>
       </c>
@@ -7364,7 +7364,7 @@
         <v>3.6040000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>132</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>3.6669999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>132</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>3.806</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>3.8879999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>132</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>4.1429999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>132</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>5.6070000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>133</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>3.9380000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>133</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>3.867</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>133</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>3.9780000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>133</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>4.0350000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>133</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>2.653</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>133</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>3.012</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>134</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>134</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>4.2030000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>134</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>3.9649999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>134</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>2.7109999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>134</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>3.1219999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>134</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>3.3889999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>135</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>3.3730000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>135</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>3.6019999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>135</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>4.867</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>135</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>3.8439999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>135</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>3.8719999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>135</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>4.0620000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>136</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>136</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>3.6040000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>136</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>3.7210000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>4.1619999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>136</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>4.226</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>137</v>
       </c>
@@ -8774,7 +8774,7 @@
         <v>4.0979999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>137</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>4.1769999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>137</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>2.794</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>2.9740000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>137</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>3.137</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>137</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>3.2189999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>138</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>5.1280000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>138</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>4.2880000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>138</v>
       </c>
@@ -9150,7 +9150,7 @@
         <v>2.726</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>138</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>2.988</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>138</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>3.1520000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>138</v>
       </c>
@@ -9289,7 +9289,7 @@
         <v>4.8860000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>139</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>3.3959999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>3.4580000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>139</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>3.673</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>139</v>
       </c>
@@ -9477,7 +9477,7 @@
         <v>3.7949999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>139</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>3.9980000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>139</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>3.7309999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>140</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>2.7240000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>140</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>2.923</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>140</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>3.1829999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>140</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>3.3039999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>140</v>
       </c>
@@ -9806,7 +9806,7 @@
         <v>3.448</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>140</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>3.694</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>141</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>141</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>3.2570000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>141</v>
       </c>
@@ -9994,7 +9994,7 @@
         <v>2.6230000000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>141</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>2.9449999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>3.2879999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>141</v>
       </c>
@@ -10135,7 +10135,7 @@
         <v>3.3719999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>231</v>
       </c>
@@ -10182,7 +10182,7 @@
         <v>2.8919999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>231</v>
       </c>
@@ -10229,7 +10229,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>231</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>3.3460000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>231</v>
       </c>
@@ -10337,24 +10337,24 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.375" customWidth="1"/>
+    <col min="2" max="3" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="27.875" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
+    <col min="6" max="7" width="17.625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
     <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
     <col min="12" max="12" width="26.5" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="19.375" customWidth="1"/>
+    <col min="14" max="14" width="16.125" customWidth="1"/>
+    <col min="15" max="15" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>143</v>
       </c>
@@ -10401,7 +10401,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>3.5750000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>157</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>2.6880000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>157</v>
       </c>
@@ -10542,7 +10542,7 @@
         <v>3.153</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>3.4020000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>157</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>3.508</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>157</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>132</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>132</v>
       </c>
@@ -10777,7 +10777,7 @@
         <v>5.3769999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>132</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>5.891</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>3.2719999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>132</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>3.407</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>132</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>3.6659999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>133</v>
       </c>
@@ -11012,7 +11012,7 @@
         <v>4.3730000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>133</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>4.4470000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>133</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>4.5439999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>133</v>
       </c>
@@ -11153,7 +11153,7 @@
         <v>4.3819999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>133</v>
       </c>
@@ -11200,7 +11200,7 @@
         <v>2.8260000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>133</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>3.258</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>134</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>3.0169999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>134</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>134</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>3.2759999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>134</v>
       </c>
@@ -11435,7 +11435,7 @@
         <v>3.4830000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>134</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>3.6589999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>134</v>
       </c>
@@ -11529,7 +11529,7 @@
         <v>3.8580000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>135</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>3.472</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>135</v>
       </c>
@@ -11623,7 +11623,7 @@
         <v>3.637</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>135</v>
       </c>
@@ -11670,7 +11670,7 @@
         <v>3.7669999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>135</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>3.9710000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>135</v>
       </c>
@@ -11764,7 +11764,7 @@
         <v>4.1529999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>135</v>
       </c>
@@ -11811,7 +11811,7 @@
         <v>5.4630000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>136</v>
       </c>
@@ -11858,7 +11858,7 @@
         <v>3.996</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>136</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>4.3040000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>136</v>
       </c>
@@ -11934,7 +11934,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
@@ -11981,7 +11981,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>2.8039999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>136</v>
       </c>
@@ -12075,7 +12075,7 @@
         <v>3.0489999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>137</v>
       </c>
@@ -12122,7 +12122,7 @@
         <v>5.5620000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>137</v>
       </c>
@@ -12169,7 +12169,7 @@
         <v>6.29</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>137</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>3.2559999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -12263,7 +12263,7 @@
         <v>3.4390000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>137</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>3.6160000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>137</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>138</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>3.3140000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>138</v>
       </c>
@@ -12451,7 +12451,7 @@
         <v>3.5379999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>138</v>
       </c>
@@ -12498,7 +12498,7 @@
         <v>3.6480000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>138</v>
       </c>
@@ -12545,7 +12545,7 @@
         <v>3.8450000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>138</v>
       </c>
@@ -12592,7 +12592,7 @@
         <v>4.0869999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>138</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>4.2270000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>139</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>4.0279999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
@@ -12733,7 +12733,7 @@
         <v>3.6539999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>139</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>3.617</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>139</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>139</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>3.9969999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>139</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>4.1989999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>140</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>3.8889999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>140</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>4.0709999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>140</v>
       </c>
@@ -13062,7 +13062,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>140</v>
       </c>
@@ -13109,7 +13109,7 @@
         <v>4.367</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>140</v>
       </c>
@@ -13156,7 +13156,7 @@
         <v>5.3659999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>140</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>4.1059999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>141</v>
       </c>
@@ -13250,7 +13250,7 @@
         <v>3.677</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>141</v>
       </c>
@@ -13297,7 +13297,7 @@
         <v>3.8279999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>141</v>
       </c>
@@ -13344,7 +13344,7 @@
         <v>3.9550000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>141</v>
       </c>
@@ -13391,7 +13391,7 @@
         <v>3.605</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -13438,7 +13438,7 @@
         <v>3.077</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>141</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>3.3730000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>231</v>
       </c>
@@ -13532,7 +13532,7 @@
         <v>3.9849999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>231</v>
       </c>
@@ -13579,7 +13579,7 @@
         <v>3.8980000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>231</v>
       </c>
@@ -13626,7 +13626,7 @@
         <v>3.6930000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>231</v>
       </c>
@@ -13679,15 +13679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8DF4565409F7A498078360796F26CA9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d9fe6ba3ad0296993fdf9ca86fb8ec6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="13928eb9-0d8a-4018-8962-fa9e89967672" xmlns:ns3="d960e8a8-69e2-40a4-bb78-08ff18f8bb2f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84c00418da9684fb2e9f40c453441992" ns2:_="" ns3:_="">
     <xsd:import namespace="13928eb9-0d8a-4018-8962-fa9e89967672"/>
@@ -13942,15 +13933,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C7EE5A2-8461-4909-A45F-0A6C43DF2417}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209E5E74-AAAA-4AAD-832B-22F4FC51D717}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13967,4 +13959,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C7EE5A2-8461-4909-A45F-0A6C43DF2417}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>